<commit_message>
Added exclusion option to sheet2
</commit_message>
<xml_diff>
--- a/swedr_excel_template.xlsx
+++ b/swedr_excel_template.xlsx
@@ -11,7 +11,7 @@
     <sheet name="variable_attributes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">variable_attributes!$A$1:$F$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">variable_attributes!$A$1:$G$2</definedName>
     <definedName name="_xlnm.Extract" localSheetId="1">variable_attributes!$A$2</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>dia_codes</t>
   </si>
@@ -53,9 +53,6 @@
     <t>after_time1</t>
   </si>
   <si>
-    <t>after_time2</t>
-  </si>
-  <si>
     <t>-Inf</t>
   </si>
   <si>
@@ -63,6 +60,12 @@
   </si>
   <si>
     <t>name_of_code</t>
+  </si>
+  <si>
+    <t>after_time12</t>
+  </si>
+  <si>
+    <t>exclude_outside</t>
   </si>
 </sst>
 </file>
@@ -162,15 +165,16 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F24" totalsRowShown="0">
-  <autoFilter ref="A1:F24"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:G24" totalsRowShown="0">
+  <autoFilter ref="A1:G24"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="variable_name"/>
     <tableColumn id="2" name="relationship"/>
     <tableColumn id="3" name="before_time1"/>
     <tableColumn id="4" name="before_time2"/>
     <tableColumn id="5" name="after_time1"/>
-    <tableColumn id="6" name="after_time2"/>
+    <tableColumn id="7" name="after_time12"/>
+    <tableColumn id="6" name="exclude_outside"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -524,10 +528,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="167" spans="1:5">
@@ -553,19 +557,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.83203125" customWidth="1"/>
     <col min="2" max="2" width="13.5" customWidth="1"/>
     <col min="3" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="6" width="13.33203125" customWidth="1"/>
+    <col min="5" max="7" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -582,10 +588,13 @@
         <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="2">
         <f t="array" ref="A2">INDEX(code_entry!$C$1:$C$150, MATCH(0, COUNTIF(variable_attributes!$A$1:A1, code_entry!$C$1:$C$150), 0))</f>
         <v>0</v>
@@ -594,7 +603,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -604,6 +613,9 @@
       </c>
       <c r="F2" t="s">
         <v>5</v>
+      </c>
+      <c r="G2" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>